<commit_message>
added cumulative capacity plot to electricity supply indicator
</commit_message>
<xml_diff>
--- a/dashboard/Data/Renewables.xlsx
+++ b/dashboard/Data/Renewables.xlsx
@@ -75,7 +75,7 @@
     <t>PWR_BIO_001</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>Source</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>